<commit_message>
[14.0][REF] account_statement_import_txt_xlsx: refactor for easy to hook
</commit_message>
<xml_diff>
--- a/account_statement_import_txt_xlsx/tests/fixtures/sample_statement_en.xlsx
+++ b/account_statement_import_txt_xlsx/tests/fixtures/sample_statement_en.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -43,6 +43,15 @@
     <t xml:space="preserve">Bank Account</t>
   </si>
   <si>
+    <t xml:space="preserve">Bank Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Your best supplier on 12/15/2018</t>
   </si>
   <si>
@@ -53,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REF1812001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fines</t>
   </si>
   <si>
     <t xml:space="preserve">Your payment on 12/15/2018</t>
@@ -71,7 +89,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -157,36 +175,32 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,16 +225,25 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>43449</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>-33.5</v>
@@ -229,10 +252,19 @@
         <v>0</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,10 +272,10 @@
         <v>43449</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1525</v>
@@ -252,7 +284,7 @@
         <v>1000</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -260,8 +292,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>